<commit_message>
Modification of the parameters for sensitivity (weibull lifetime, RR, price of metals)
</commit_message>
<xml_diff>
--- a/Recycling/Recycling parameters.xlsx
+++ b/Recycling/Recycling parameters.xlsx
@@ -1,45 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10608728_polimi_it/Documents/Documenti/GitHub/GreenTechs/Recycling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documenti\GitHub\GreenTechs\Recycling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{F49D9DD3-0A2E-4A92-BA0B-45BDAE5ED3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D16574E-C5B6-4DEE-972A-5C3C29EA9F8A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41A974B-4916-43F5-9EC2-91B9CEA99C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" firstSheet="1" activeTab="1" xr2:uid="{AC6E99B7-2CCE-416B-9DC6-70CD92A8276E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{AC6E99B7-2CCE-416B-9DC6-70CD92A8276E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sector Index" sheetId="14" r:id="rId1"/>
-    <sheet name="USD to EURO" sheetId="13" r:id="rId2"/>
-    <sheet name="Weibull" sheetId="2" r:id="rId3"/>
-    <sheet name="S" sheetId="3" r:id="rId4"/>
-    <sheet name="CR" sheetId="4" r:id="rId5"/>
-    <sheet name="DR" sheetId="5" r:id="rId6"/>
-    <sheet name="RE" sheetId="6" r:id="rId7"/>
-    <sheet name="RR" sheetId="7" r:id="rId8"/>
-    <sheet name="Inventory_comp" sheetId="11" r:id="rId9"/>
-    <sheet name="Inventory_mat" sheetId="12" r:id="rId10"/>
-    <sheet name="price materials" sheetId="16" r:id="rId11"/>
+    <sheet name="region" sheetId="17" r:id="rId2"/>
+    <sheet name="USD to EURO" sheetId="13" r:id="rId3"/>
+    <sheet name="Weibull" sheetId="2" r:id="rId4"/>
+    <sheet name="S" sheetId="3" r:id="rId5"/>
+    <sheet name="CR" sheetId="4" r:id="rId6"/>
+    <sheet name="DR" sheetId="5" r:id="rId7"/>
+    <sheet name="RE" sheetId="6" r:id="rId8"/>
+    <sheet name="RR" sheetId="18" r:id="rId9"/>
+    <sheet name="Inventory_comp" sheetId="11" r:id="rId10"/>
+    <sheet name="Inventory_mat" sheetId="12" r:id="rId11"/>
+    <sheet name="price materials" sheetId="16" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -53,10 +43,19 @@
   <commentList>
     <comment ref="E4" authorId="0" shapeId="0" xr:uid="{EA1C9821-13DA-41E5-9D13-34457A68D50C}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Allora qui ho preso quello del Cu nei wires delle WT percentuale molto simile ai PV dopo ragiono se si può fare meglio</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="249">
   <si>
     <t>lambda</t>
   </si>
@@ -799,6 +798,18 @@
   </si>
   <si>
     <t>Copper</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>EU27+UK</t>
+  </si>
+  <si>
+    <t>RoW</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -880,9 +891,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -920,7 +931,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1026,7 +1037,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1168,7 +1179,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2263,6 +2274,88 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9FFD70-C54F-44B1-9684-4988A1F88D7D}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0.11537368682717926</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>5.2634440430628648E-2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.26872981670314472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>5.5734566509897124E-2</v>
+      </c>
+      <c r="C5">
+        <v>5.5734566509897124E-2</v>
+      </c>
+      <c r="D5">
+        <v>6.0498990481684452E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49257BDC-919A-4399-93A8-CC4D137B2BDF}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2366,12 +2459,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D81820-136A-4103-B600-42B0112B1E96}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2393,15 +2486,13 @@
         <v>137</v>
       </c>
       <c r="B2">
-        <f>C2*(1-0.1)</f>
-        <v>44.1</v>
+        <v>39.326999999999998</v>
       </c>
       <c r="C2" s="5">
         <v>49</v>
       </c>
       <c r="D2">
-        <f>C2*(1+0.1)</f>
-        <v>53.900000000000006</v>
+        <v>66.2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -2409,15 +2500,13 @@
         <v>74</v>
       </c>
       <c r="B3">
-        <f>C3*(1-0.1)</f>
-        <v>234</v>
+        <v>177</v>
       </c>
       <c r="C3" s="5">
         <v>260</v>
       </c>
       <c r="D3">
-        <f>C3*(1+0.1)</f>
-        <v>286</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -2425,15 +2514,13 @@
         <v>244</v>
       </c>
       <c r="B4">
-        <f>C4*(1-0.1)</f>
-        <v>5.5529999999999999</v>
+        <v>4.8678999999999997</v>
       </c>
       <c r="C4" s="5">
         <v>6.17</v>
       </c>
       <c r="D4">
-        <f>C4*(1+0.1)</f>
-        <v>6.7870000000000008</v>
+        <v>9.3170000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -2441,15 +2528,13 @@
         <v>191</v>
       </c>
       <c r="B5">
-        <f>C5*(1-0.1)</f>
-        <v>1.9710000000000001</v>
+        <v>1.6819999999999999</v>
       </c>
       <c r="C5">
         <v>2.19</v>
       </c>
       <c r="D5">
-        <f>C5*(1+0.1)</f>
-        <v>2.4090000000000003</v>
+        <v>3.645</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -2470,10 +2555,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB99539-CC9D-4EB2-9CEF-901856066E73}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E3B2D2-0DE2-4163-BA20-6ABECB371F4E}">
   <dimension ref="A1:CX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -3097,12 +3217,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C12DD5-DBE8-4ECA-8D71-7BDA7AF5A766}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3128,12 +3248,10 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <f>C3- (0.1*C3)</f>
-        <v>20.25</v>
+        <v>17</v>
       </c>
       <c r="D2">
-        <f>D3- (0.1*D3)</f>
-        <v>20.16</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -3158,12 +3276,10 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <f>C3+(C3*0.1)</f>
-        <v>24.75</v>
+        <v>30</v>
       </c>
       <c r="D4">
-        <f>D3+(D3*0.1)</f>
-        <v>24.639999999999997</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -3174,12 +3290,10 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <f>C6- (0.1*C6)</f>
-        <v>20.25</v>
+        <v>17</v>
       </c>
       <c r="D5">
-        <f>D6- (0.1*D6)</f>
-        <v>20.16</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -3204,12 +3318,10 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <f>C6+(C6*0.1)</f>
-        <v>24.75</v>
+        <v>30</v>
       </c>
       <c r="D7">
-        <f>D6+(D6*0.1)</f>
-        <v>24.639999999999997</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -3220,12 +3332,10 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <f>C9- (0.1*C9)</f>
-        <v>22.5</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <f>D9- (0.1*D9)</f>
-        <v>4.8600000000000003</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -3250,12 +3360,10 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <f>C9+(C9*0.1)</f>
-        <v>27.5</v>
+        <v>42</v>
       </c>
       <c r="D10">
-        <f>D9+(D9*0.1)</f>
-        <v>5.94</v>
+        <v>5.4</v>
       </c>
     </row>
   </sheetData>
@@ -3263,7 +3371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D80951-6AC3-4467-ACD0-C3C680A5E3F8}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -3524,7 +3632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AA6CF8-62F9-4D8D-8F49-5ACA73129446}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3555,7 +3663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E98E62-C3BF-4DFF-BC53-14C4DB855449}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3586,7 +3694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DC0C1A-BBC4-4838-959E-FC2B382C2F16}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3629,164 +3737,4231 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C841F7-A404-465C-B615-CD7E5C0C1A29}">
-  <dimension ref="A1:E12"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C8A0BA-7516-44AA-95A8-AE02F79FDD83}">
+  <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1" t="s">
+        <v>242</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B2">
-        <v>0.01</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0.5</v>
-      </c>
-      <c r="E2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>242</v>
+      <c r="F2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2000</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>0.01</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0.5</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>243</v>
+        <v>0.01</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3">
+        <v>0.01</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2001</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C12" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9FFD70-C54F-44B1-9684-4988A1F88D7D}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>0.11537368682717926</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>5.2634440430628648E-2</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0.26872981670314472</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
+        <v>0.01</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <v>0.01</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2002</v>
       </c>
       <c r="B5">
-        <v>5.5734566509897124E-2</v>
+        <v>0.01</v>
       </c>
       <c r="C5">
-        <v>5.5734566509897124E-2</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>6.0498990481684452E-2</v>
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>0.01</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2003</v>
+      </c>
+      <c r="B6">
+        <v>0.01</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>0.01</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+      <c r="I6">
+        <v>0.01</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2004</v>
+      </c>
+      <c r="B7">
+        <v>0.01</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>0.01</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>0.01</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2005</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>0.01</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0.5</v>
+      </c>
+      <c r="I8">
+        <v>0.01</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2006</v>
+      </c>
+      <c r="B9">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <v>0.01</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>0.01</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2007</v>
+      </c>
+      <c r="B10">
+        <v>0.01</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <v>0.01</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="I10">
+        <v>0.01</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2008</v>
+      </c>
+      <c r="B11">
+        <v>0.01</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <v>0.01</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>0.01</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2009</v>
+      </c>
+      <c r="B12">
+        <v>0.01</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+      <c r="E12">
+        <v>0.01</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+      <c r="I12">
+        <v>0.01</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2010</v>
+      </c>
+      <c r="B13">
+        <v>0.01</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
+        <v>0.01</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0.5</v>
+      </c>
+      <c r="I13">
+        <v>0.01</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2011</v>
+      </c>
+      <c r="B14">
+        <v>0.01</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+      <c r="E14">
+        <v>0.01</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
+      <c r="I14">
+        <v>0.01</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2012</v>
+      </c>
+      <c r="B15">
+        <v>0.01</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.5</v>
+      </c>
+      <c r="E15">
+        <v>0.01</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0.5</v>
+      </c>
+      <c r="I15">
+        <v>0.01</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2013</v>
+      </c>
+      <c r="B16">
+        <v>0.01</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+      <c r="E16">
+        <v>0.01</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0.5</v>
+      </c>
+      <c r="I16">
+        <v>0.01</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2014</v>
+      </c>
+      <c r="B17">
+        <v>0.01</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+      <c r="E17">
+        <v>0.01</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="I17">
+        <v>0.01</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2015</v>
+      </c>
+      <c r="B18">
+        <v>0.01</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+      <c r="E18">
+        <v>0.01</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+      <c r="I18">
+        <v>0.01</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2016</v>
+      </c>
+      <c r="B19">
+        <v>0.01</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
+      <c r="E19">
+        <v>0.01</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>0.01</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2017</v>
+      </c>
+      <c r="B20">
+        <v>0.01</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20">
+        <v>0.01</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0.5</v>
+      </c>
+      <c r="I20">
+        <v>0.01</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2018</v>
+      </c>
+      <c r="B21">
+        <v>0.01</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>0.01</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0.5</v>
+      </c>
+      <c r="I21">
+        <v>0.01</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2019</v>
+      </c>
+      <c r="B22">
+        <v>0.01</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.5</v>
+      </c>
+      <c r="E22">
+        <v>0.01</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0.5</v>
+      </c>
+      <c r="I22">
+        <v>0.01</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2020</v>
+      </c>
+      <c r="B23">
+        <v>0.01</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.5</v>
+      </c>
+      <c r="E23">
+        <v>0.01</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0.5</v>
+      </c>
+      <c r="I23">
+        <v>0.01</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2021</v>
+      </c>
+      <c r="B24">
+        <v>0.01</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+      <c r="E24">
+        <v>0.01</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0.5</v>
+      </c>
+      <c r="I24">
+        <v>0.01</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2022</v>
+      </c>
+      <c r="B25">
+        <v>0.01</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.5</v>
+      </c>
+      <c r="E25">
+        <v>0.01</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0.5</v>
+      </c>
+      <c r="I25">
+        <v>0.01</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B26">
+        <v>0.01</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0.5</v>
+      </c>
+      <c r="E26">
+        <v>0.01</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0.5</v>
+      </c>
+      <c r="I26">
+        <v>0.01</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2024</v>
+      </c>
+      <c r="B27">
+        <v>0.01</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0.5</v>
+      </c>
+      <c r="E27">
+        <v>0.01</v>
+      </c>
+      <c r="F27">
+        <v>2.6829436724348201E-2</v>
+      </c>
+      <c r="G27">
+        <v>2.78975719889193E-2</v>
+      </c>
+      <c r="H27">
+        <v>0.51539085595733203</v>
+      </c>
+      <c r="I27">
+        <v>3.2699422828663602E-2</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>2025</v>
+      </c>
+      <c r="B28">
+        <v>0.01</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0.5</v>
+      </c>
+      <c r="E28">
+        <v>0.01</v>
+      </c>
+      <c r="F28">
+        <v>5.4034630351002103E-2</v>
+      </c>
+      <c r="G28">
+        <v>5.6669155306979697E-2</v>
+      </c>
+      <c r="H28">
+        <v>0.53063716240803904</v>
+      </c>
+      <c r="I28">
+        <v>5.52052584473973E-2</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2026</v>
+      </c>
+      <c r="B29">
+        <v>0.01</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+      <c r="E29">
+        <v>0.01</v>
+      </c>
+      <c r="F29">
+        <v>8.0309953679422896E-2</v>
+      </c>
+      <c r="G29">
+        <v>8.4496543044626907E-2</v>
+      </c>
+      <c r="H29">
+        <v>0.54560462072177196</v>
+      </c>
+      <c r="I29">
+        <v>7.7093774616426303E-2</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>2027</v>
+      </c>
+      <c r="B30">
+        <v>0.01</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0.5</v>
+      </c>
+      <c r="E30">
+        <v>0.01</v>
+      </c>
+      <c r="F30">
+        <v>0.104349779509071</v>
+      </c>
+      <c r="G30">
+        <v>0.109561528292306</v>
+      </c>
+      <c r="H30">
+        <v>0.56015893226818303</v>
+      </c>
+      <c r="I30">
+        <v>9.7941239095975796E-2</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2028</v>
+      </c>
+      <c r="B31">
+        <v>0.01</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+      <c r="E31">
+        <v>0.01</v>
+      </c>
+      <c r="F31">
+        <v>0.12484848063940999</v>
+      </c>
+      <c r="G31">
+        <v>0.13004590414046499</v>
+      </c>
+      <c r="H31">
+        <v>0.57416579841692394</v>
+      </c>
+      <c r="I31">
+        <v>0.11732391964627099</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>2029</v>
+      </c>
+      <c r="B32">
+        <v>0.01</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <v>0.01</v>
+      </c>
+      <c r="F32">
+        <v>0.140500429869899</v>
+      </c>
+      <c r="G32">
+        <v>0.14413146367954699</v>
+      </c>
+      <c r="H32">
+        <v>0.58749092053764496</v>
+      </c>
+      <c r="I32">
+        <v>0.13481808402753701</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>2030</v>
+      </c>
+      <c r="B33">
+        <v>0.01</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0.5</v>
+      </c>
+      <c r="E33">
+        <v>0.01</v>
+      </c>
+      <c r="F33">
+        <v>0.15</v>
+      </c>
+      <c r="G33">
+        <v>0.15</v>
+      </c>
+      <c r="H33">
+        <v>0.6</v>
+      </c>
+      <c r="I33">
+        <v>0.15</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
+        <v>2031</v>
+      </c>
+      <c r="B34">
+        <v>0.01</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0.5</v>
+      </c>
+      <c r="E34">
+        <v>0.01</v>
+      </c>
+      <c r="F34">
+        <v>0.15562490890268599</v>
+      </c>
+      <c r="G34">
+        <v>0.151073409636411</v>
+      </c>
+      <c r="H34">
+        <v>0.61202891359918199</v>
+      </c>
+      <c r="I34">
+        <v>0.16345710615148001</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2032</v>
+      </c>
+      <c r="B35">
+        <v>0.01</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0.5</v>
+      </c>
+      <c r="E35">
+        <v>0.01</v>
+      </c>
+      <c r="F35">
+        <v>0.160568314486672</v>
+      </c>
+      <c r="G35">
+        <v>0.15199580039314001</v>
+      </c>
+      <c r="H35">
+        <v>0.62398631471013799</v>
+      </c>
+      <c r="I35">
+        <v>0.17610589423380901</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
+        <v>2033</v>
+      </c>
+      <c r="B36">
+        <v>0.01</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.5</v>
+      </c>
+      <c r="E36">
+        <v>0.01</v>
+      </c>
+      <c r="F36">
+        <v>0.16489774960502601</v>
+      </c>
+      <c r="G36">
+        <v>0.15278228226528301</v>
+      </c>
+      <c r="H36">
+        <v>0.63584706957214998</v>
+      </c>
+      <c r="I36">
+        <v>0.188016211753221</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>2034</v>
+      </c>
+      <c r="B37">
+        <v>0.01</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0.5</v>
+      </c>
+      <c r="E37">
+        <v>0.01</v>
+      </c>
+      <c r="F37">
+        <v>0.16868074711081801</v>
+      </c>
+      <c r="G37">
+        <v>0.15344796524793899</v>
+      </c>
+      <c r="H37">
+        <v>0.64758604442449696</v>
+      </c>
+      <c r="I37">
+        <v>0.19925790621595399</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
+        <v>2035</v>
+      </c>
+      <c r="B38">
+        <v>0.01</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0.5</v>
+      </c>
+      <c r="E38">
+        <v>0.01</v>
+      </c>
+      <c r="F38">
+        <v>0.17198483985711799</v>
+      </c>
+      <c r="G38">
+        <v>0.15400795933620501</v>
+      </c>
+      <c r="H38">
+        <v>0.65917810550645795</v>
+      </c>
+      <c r="I38">
+        <v>0.20990082512824301</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>2036</v>
+      </c>
+      <c r="B39">
+        <v>0.01</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0.5</v>
+      </c>
+      <c r="E39">
+        <v>0.01</v>
+      </c>
+      <c r="F39">
+        <v>0.174877560696996</v>
+      </c>
+      <c r="G39">
+        <v>0.15447737452517901</v>
+      </c>
+      <c r="H39">
+        <v>0.67059811905731403</v>
+      </c>
+      <c r="I39">
+        <v>0.220014815996325</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" s="3">
+        <v>2037</v>
+      </c>
+      <c r="B40">
+        <v>0.01</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0.5</v>
+      </c>
+      <c r="E40">
+        <v>0.01</v>
+      </c>
+      <c r="F40">
+        <v>0.17742644248352099</v>
+      </c>
+      <c r="G40">
+        <v>0.15487132080995999</v>
+      </c>
+      <c r="H40">
+        <v>0.68182095131634401</v>
+      </c>
+      <c r="I40">
+        <v>0.22966972632643501</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>2038</v>
+      </c>
+      <c r="B41">
+        <v>0.01</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0.5</v>
+      </c>
+      <c r="E41">
+        <v>0.01</v>
+      </c>
+      <c r="F41">
+        <v>0.17969901806976399</v>
+      </c>
+      <c r="G41">
+        <v>0.155204908185644</v>
+      </c>
+      <c r="H41">
+        <v>0.69282146852283</v>
+      </c>
+      <c r="I41">
+        <v>0.238935403624811</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42" s="3">
+        <v>2039</v>
+      </c>
+      <c r="B42">
+        <v>0.01</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0.5</v>
+      </c>
+      <c r="E42">
+        <v>0.01</v>
+      </c>
+      <c r="F42">
+        <v>0.18176282030879301</v>
+      </c>
+      <c r="G42">
+        <v>0.155493246647331</v>
+      </c>
+      <c r="H42">
+        <v>0.70357453691604899</v>
+      </c>
+      <c r="I42">
+        <v>0.24788169539768901</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>2040</v>
+      </c>
+      <c r="B43">
+        <v>0.01</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0.5</v>
+      </c>
+      <c r="E43">
+        <v>0.01</v>
+      </c>
+      <c r="F43">
+        <v>0.18368538205367901</v>
+      </c>
+      <c r="G43">
+        <v>0.15575144619011699</v>
+      </c>
+      <c r="H43">
+        <v>0.71405502273528298</v>
+      </c>
+      <c r="I43">
+        <v>0.25657844915130301</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" s="3">
+        <v>2041</v>
+      </c>
+      <c r="B44">
+        <v>0.01</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0.5</v>
+      </c>
+      <c r="E44">
+        <v>0.01</v>
+      </c>
+      <c r="F44">
+        <v>0.18553423615749201</v>
+      </c>
+      <c r="G44">
+        <v>0.15599461680910101</v>
+      </c>
+      <c r="H44">
+        <v>0.72423779221981099</v>
+      </c>
+      <c r="I44">
+        <v>0.265095512391892</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>2042</v>
+      </c>
+      <c r="B45">
+        <v>0.01</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.5</v>
+      </c>
+      <c r="E45">
+        <v>0.01</v>
+      </c>
+      <c r="F45">
+        <v>0.18737691547329999</v>
+      </c>
+      <c r="G45">
+        <v>0.15623786849938101</v>
+      </c>
+      <c r="H45">
+        <v>0.73409771160891402</v>
+      </c>
+      <c r="I45">
+        <v>0.27350273262569103</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46" s="3">
+        <v>2043</v>
+      </c>
+      <c r="B46">
+        <v>0.01</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0.5</v>
+      </c>
+      <c r="E46">
+        <v>0.01</v>
+      </c>
+      <c r="F46">
+        <v>0.18928095285417501</v>
+      </c>
+      <c r="G46">
+        <v>0.15649631125605301</v>
+      </c>
+      <c r="H46">
+        <v>0.74360964714187106</v>
+      </c>
+      <c r="I46">
+        <v>0.281869957358937</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>2044</v>
+      </c>
+      <c r="B47">
+        <v>0.01</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0.5</v>
+      </c>
+      <c r="E47">
+        <v>0.01</v>
+      </c>
+      <c r="F47">
+        <v>0.19131388115318501</v>
+      </c>
+      <c r="G47">
+        <v>0.156785055074218</v>
+      </c>
+      <c r="H47">
+        <v>0.752748465057962</v>
+      </c>
+      <c r="I47">
+        <v>0.29026703409786497</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
+        <v>2045</v>
+      </c>
+      <c r="B48">
+        <v>0.01</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0.5</v>
+      </c>
+      <c r="E48">
+        <v>0.01</v>
+      </c>
+      <c r="F48">
+        <v>0.1935432332234</v>
+      </c>
+      <c r="G48">
+        <v>0.15711920994897099</v>
+      </c>
+      <c r="H48">
+        <v>0.76148903159646597</v>
+      </c>
+      <c r="I48">
+        <v>0.29876381034871202</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2046</v>
+      </c>
+      <c r="B49">
+        <v>0.01</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0.5</v>
+      </c>
+      <c r="E49">
+        <v>0.01</v>
+      </c>
+      <c r="F49">
+        <v>0.19603654191789099</v>
+      </c>
+      <c r="G49">
+        <v>0.15751388587541101</v>
+      </c>
+      <c r="H49">
+        <v>0.76980621299666596</v>
+      </c>
+      <c r="I49">
+        <v>0.30743013361771399</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
+        <v>2047</v>
+      </c>
+      <c r="B50">
+        <v>0.01</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0.5</v>
+      </c>
+      <c r="E50">
+        <v>0.01</v>
+      </c>
+      <c r="F50">
+        <v>0.198861340089727</v>
+      </c>
+      <c r="G50">
+        <v>0.15798419284863599</v>
+      </c>
+      <c r="H50">
+        <v>0.77767487549783798</v>
+      </c>
+      <c r="I50">
+        <v>0.31633585141110798</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>2048</v>
+      </c>
+      <c r="B51">
+        <v>0.01</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0.5</v>
+      </c>
+      <c r="E51">
+        <v>0.01</v>
+      </c>
+      <c r="F51">
+        <v>0.20208516059197701</v>
+      </c>
+      <c r="G51">
+        <v>0.158545240863744</v>
+      </c>
+      <c r="H51">
+        <v>0.78506988533926503</v>
+      </c>
+      <c r="I51">
+        <v>0.32555081123512902</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A52" s="3">
+        <v>2049</v>
+      </c>
+      <c r="B52">
+        <v>0.01</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0.5</v>
+      </c>
+      <c r="E52">
+        <v>0.01</v>
+      </c>
+      <c r="F52">
+        <v>0.205775536277711</v>
+      </c>
+      <c r="G52">
+        <v>0.159212139915833</v>
+      </c>
+      <c r="H52">
+        <v>0.791966108760225</v>
+      </c>
+      <c r="I52">
+        <v>0.335144860596014</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>2050</v>
+      </c>
+      <c r="B53">
+        <v>0.01</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0.5</v>
+      </c>
+      <c r="E53">
+        <v>0.01</v>
+      </c>
+      <c r="F53">
+        <v>0.21</v>
+      </c>
+      <c r="G53">
+        <v>0.16</v>
+      </c>
+      <c r="H53">
+        <v>0.798338412</v>
+      </c>
+      <c r="I53">
+        <v>0.34518784699999999</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A54" s="3">
+        <v>2051</v>
+      </c>
+      <c r="B54">
+        <v>0.01</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0.5</v>
+      </c>
+      <c r="E54">
+        <v>0.01</v>
+      </c>
+      <c r="F54">
+        <v>0.214730543551401</v>
+      </c>
+      <c r="G54">
+        <v>0.161205463525535</v>
+      </c>
+      <c r="H54">
+        <v>0.80443750672606695</v>
+      </c>
+      <c r="I54">
+        <v>0.35549176654071601</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>2052</v>
+      </c>
+      <c r="B55">
+        <v>0.01</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0.5</v>
+      </c>
+      <c r="E55">
+        <v>0.01</v>
+      </c>
+      <c r="F55">
+        <v>0.21989162210947899</v>
+      </c>
+      <c r="G55">
+        <v>0.16310912783243101</v>
+      </c>
+      <c r="H55">
+        <v>0.81052771724911998</v>
+      </c>
+      <c r="I55">
+        <v>0.36582228932800898</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A56" s="3">
+        <v>2053</v>
+      </c>
+      <c r="B56">
+        <v>0.01</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0.5</v>
+      </c>
+      <c r="E56">
+        <v>0.01</v>
+      </c>
+      <c r="F56">
+        <v>0.225479463604806</v>
+      </c>
+      <c r="G56">
+        <v>0.165702035311838</v>
+      </c>
+      <c r="H56">
+        <v>0.81660432877325995</v>
+      </c>
+      <c r="I56">
+        <v>0.37617977389243401</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>2054</v>
+      </c>
+      <c r="B57">
+        <v>0.01</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0.5</v>
+      </c>
+      <c r="E57">
+        <v>0.01</v>
+      </c>
+      <c r="F57">
+        <v>0.231490295967957</v>
+      </c>
+      <c r="G57">
+        <v>0.168975228354907</v>
+      </c>
+      <c r="H57">
+        <v>0.82266262650259003</v>
+      </c>
+      <c r="I57">
+        <v>0.38656457876454797</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A58" s="3">
+        <v>2055</v>
+      </c>
+      <c r="B58">
+        <v>0.01</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0.5</v>
+      </c>
+      <c r="E58">
+        <v>0.01</v>
+      </c>
+      <c r="F58">
+        <v>0.23792034712950599</v>
+      </c>
+      <c r="G58">
+        <v>0.172919749352788</v>
+      </c>
+      <c r="H58">
+        <v>0.82869789564121099</v>
+      </c>
+      <c r="I58">
+        <v>0.39697706247490799</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>2056</v>
+      </c>
+      <c r="B59">
+        <v>0.01</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0.5</v>
+      </c>
+      <c r="E59">
+        <v>0.01</v>
+      </c>
+      <c r="F59">
+        <v>0.24476584502002599</v>
+      </c>
+      <c r="G59">
+        <v>0.17752664069663401</v>
+      </c>
+      <c r="H59">
+        <v>0.83470542139322301</v>
+      </c>
+      <c r="I59">
+        <v>0.40741758355407098</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A60" s="3">
+        <v>2057</v>
+      </c>
+      <c r="B60">
+        <v>0.01</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0.5</v>
+      </c>
+      <c r="E60">
+        <v>0.01</v>
+      </c>
+      <c r="F60">
+        <v>0.25202301757009299</v>
+      </c>
+      <c r="G60">
+        <v>0.182786944777594</v>
+      </c>
+      <c r="H60">
+        <v>0.84068048896272896</v>
+      </c>
+      <c r="I60">
+        <v>0.41788650053259202</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+      <c r="M60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>2058</v>
+      </c>
+      <c r="B61">
+        <v>0.01</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0.5</v>
+      </c>
+      <c r="E61">
+        <v>0.01</v>
+      </c>
+      <c r="F61">
+        <v>0.25968809271027998</v>
+      </c>
+      <c r="G61">
+        <v>0.18869170398682</v>
+      </c>
+      <c r="H61">
+        <v>0.84661838355383001</v>
+      </c>
+      <c r="I61">
+        <v>0.42838417194102801</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>1</v>
+      </c>
+      <c r="M61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A62" s="3">
+        <v>2059</v>
+      </c>
+      <c r="B62">
+        <v>0.01</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0.5</v>
+      </c>
+      <c r="E62">
+        <v>0.01</v>
+      </c>
+      <c r="F62">
+        <v>0.26775729837116102</v>
+      </c>
+      <c r="G62">
+        <v>0.19523196071546201</v>
+      </c>
+      <c r="H62">
+        <v>0.85251439037062704</v>
+      </c>
+      <c r="I62">
+        <v>0.43891095630993598</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="M62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>2060</v>
+      </c>
+      <c r="B63">
+        <v>0.01</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0.5</v>
+      </c>
+      <c r="E63">
+        <v>0.01</v>
+      </c>
+      <c r="F63">
+        <v>0.27622686248331102</v>
+      </c>
+      <c r="G63">
+        <v>0.202398757354671</v>
+      </c>
+      <c r="H63">
+        <v>0.85836379461722201</v>
+      </c>
+      <c r="I63">
+        <v>0.44946721216987301</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
+        <v>2061</v>
+      </c>
+      <c r="B64">
+        <v>0.01</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0.5</v>
+      </c>
+      <c r="E64">
+        <v>0.01</v>
+      </c>
+      <c r="F64">
+        <v>0.285093012977303</v>
+      </c>
+      <c r="G64">
+        <v>0.21018313629559801</v>
+      </c>
+      <c r="H64">
+        <v>0.864161881497716</v>
+      </c>
+      <c r="I64">
+        <v>0.460053298051395</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>2062</v>
+      </c>
+      <c r="B65">
+        <v>0.01</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0.5</v>
+      </c>
+      <c r="E65">
+        <v>0.01</v>
+      </c>
+      <c r="F65">
+        <v>0.29435197778371103</v>
+      </c>
+      <c r="G65">
+        <v>0.21857613992939501</v>
+      </c>
+      <c r="H65">
+        <v>0.86990393621621098</v>
+      </c>
+      <c r="I65">
+        <v>0.47066957248505797</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+      <c r="M65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A66" s="3">
+        <v>2063</v>
+      </c>
+      <c r="B66">
+        <v>0.01</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0.5</v>
+      </c>
+      <c r="E66">
+        <v>0.01</v>
+      </c>
+      <c r="F66">
+        <v>0.30399998483311003</v>
+      </c>
+      <c r="G66">
+        <v>0.22756881064721099</v>
+      </c>
+      <c r="H66">
+        <v>0.87558524397680904</v>
+      </c>
+      <c r="I66">
+        <v>0.48131639400142001</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="M66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>2064</v>
+      </c>
+      <c r="B67">
+        <v>0.01</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0.5</v>
+      </c>
+      <c r="E67">
+        <v>0.01</v>
+      </c>
+      <c r="F67">
+        <v>0.31403326205607401</v>
+      </c>
+      <c r="G67">
+        <v>0.23715219084019701</v>
+      </c>
+      <c r="H67">
+        <v>0.88120108998361002</v>
+      </c>
+      <c r="I67">
+        <v>0.49199412113103602</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A68" s="3">
+        <v>2065</v>
+      </c>
+      <c r="B68">
+        <v>0.01</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0.5</v>
+      </c>
+      <c r="E68">
+        <v>0.01</v>
+      </c>
+      <c r="F68">
+        <v>0.32444803738317701</v>
+      </c>
+      <c r="G68">
+        <v>0.247317322899505</v>
+      </c>
+      <c r="H68">
+        <v>0.88674675944071601</v>
+      </c>
+      <c r="I68">
+        <v>0.50270311240446397</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>2066</v>
+      </c>
+      <c r="B69">
+        <v>0.01</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0.5</v>
+      </c>
+      <c r="E69">
+        <v>0.01</v>
+      </c>
+      <c r="F69">
+        <v>0.33524053874499299</v>
+      </c>
+      <c r="G69">
+        <v>0.25805524921628598</v>
+      </c>
+      <c r="H69">
+        <v>0.89221753755222899</v>
+      </c>
+      <c r="I69">
+        <v>0.51344372635225899</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+      <c r="M69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A70" s="3">
+        <v>2067</v>
+      </c>
+      <c r="B70">
+        <v>0.01</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0.5</v>
+      </c>
+      <c r="E70">
+        <v>0.01</v>
+      </c>
+      <c r="F70">
+        <v>0.34640699407209602</v>
+      </c>
+      <c r="G70">
+        <v>0.269357012181689</v>
+      </c>
+      <c r="H70">
+        <v>0.89760870952224903</v>
+      </c>
+      <c r="I70">
+        <v>0.52421632150497899</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+      <c r="M70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>2068</v>
+      </c>
+      <c r="B71">
+        <v>0.01</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0.5</v>
+      </c>
+      <c r="E71">
+        <v>0.01</v>
+      </c>
+      <c r="F71">
+        <v>0.35794363129506002</v>
+      </c>
+      <c r="G71">
+        <v>0.281213654186867</v>
+      </c>
+      <c r="H71">
+        <v>0.90291556055487998</v>
+      </c>
+      <c r="I71">
+        <v>0.53502125639317999</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A72" s="3">
+        <v>2069</v>
+      </c>
+      <c r="B72">
+        <v>0.01</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0.5</v>
+      </c>
+      <c r="E72">
+        <v>0.01</v>
+      </c>
+      <c r="F72">
+        <v>0.369846678344459</v>
+      </c>
+      <c r="G72">
+        <v>0.29361621762297002</v>
+      </c>
+      <c r="H72">
+        <v>0.90813337585422105</v>
+      </c>
+      <c r="I72">
+        <v>0.54585888954741801</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="M72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>2070</v>
+      </c>
+      <c r="B73">
+        <v>0.01</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0.5</v>
+      </c>
+      <c r="E73">
+        <v>0.01</v>
+      </c>
+      <c r="F73">
+        <v>0.382112363150867</v>
+      </c>
+      <c r="G73">
+        <v>0.30655574488114801</v>
+      </c>
+      <c r="H73">
+        <v>0.91325744062437497</v>
+      </c>
+      <c r="I73">
+        <v>0.55672957949824997</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="M73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A74" s="3">
+        <v>2071</v>
+      </c>
+      <c r="B74">
+        <v>0.01</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0.5</v>
+      </c>
+      <c r="E74">
+        <v>0.01</v>
+      </c>
+      <c r="F74">
+        <v>0.39473691364485902</v>
+      </c>
+      <c r="G74">
+        <v>0.32002327835255301</v>
+      </c>
+      <c r="H74">
+        <v>0.91828304006944195</v>
+      </c>
+      <c r="I74">
+        <v>0.56763368477623299</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>2072</v>
+      </c>
+      <c r="B75">
+        <v>0.01</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0.5</v>
+      </c>
+      <c r="E75">
+        <v>0.01</v>
+      </c>
+      <c r="F75">
+        <v>0.40771655775700899</v>
+      </c>
+      <c r="G75">
+        <v>0.33400986042833603</v>
+      </c>
+      <c r="H75">
+        <v>0.92320545939352505</v>
+      </c>
+      <c r="I75">
+        <v>0.57857156391192299</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="M75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A76" s="3">
+        <v>2073</v>
+      </c>
+      <c r="B76">
+        <v>0.01</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0.5</v>
+      </c>
+      <c r="E76">
+        <v>0.01</v>
+      </c>
+      <c r="F76">
+        <v>0.42104752341788998</v>
+      </c>
+      <c r="G76">
+        <v>0.348506533499647</v>
+      </c>
+      <c r="H76">
+        <v>0.92801998380072503</v>
+      </c>
+      <c r="I76">
+        <v>0.58954357543587699</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>1</v>
+      </c>
+      <c r="M76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>2074</v>
+      </c>
+      <c r="B77">
+        <v>0.01</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0.5</v>
+      </c>
+      <c r="E77">
+        <v>0.01</v>
+      </c>
+      <c r="F77">
+        <v>0.43472603855807701</v>
+      </c>
+      <c r="G77">
+        <v>0.36350433995763698</v>
+      </c>
+      <c r="H77">
+        <v>0.93272189849514298</v>
+      </c>
+      <c r="I77">
+        <v>0.600550077878651</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A78" s="3">
+        <v>2075</v>
+      </c>
+      <c r="B78">
+        <v>0.01</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0.5</v>
+      </c>
+      <c r="E78">
+        <v>0.01</v>
+      </c>
+      <c r="F78">
+        <v>0.44874833110814399</v>
+      </c>
+      <c r="G78">
+        <v>0.37899432219345702</v>
+      </c>
+      <c r="H78">
+        <v>0.93730648868088096</v>
+      </c>
+      <c r="I78">
+        <v>0.61159142977080205</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+      <c r="M78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>2076</v>
+      </c>
+      <c r="B79">
+        <v>0.01</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0.5</v>
+      </c>
+      <c r="E79">
+        <v>0.01</v>
+      </c>
+      <c r="F79">
+        <v>0.46311062899866401</v>
+      </c>
+      <c r="G79">
+        <v>0.39496752259825801</v>
+      </c>
+      <c r="H79">
+        <v>0.94176903956203994</v>
+      </c>
+      <c r="I79">
+        <v>0.62266798964288705</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="M79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A80" s="3">
+        <v>2077</v>
+      </c>
+      <c r="B80">
+        <v>0.01</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0.5</v>
+      </c>
+      <c r="E80">
+        <v>0.01</v>
+      </c>
+      <c r="F80">
+        <v>0.47780916016021302</v>
+      </c>
+      <c r="G80">
+        <v>0.41141498356319101</v>
+      </c>
+      <c r="H80">
+        <v>0.94610483634272102</v>
+      </c>
+      <c r="I80">
+        <v>0.63378011602546103</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>2078</v>
+      </c>
+      <c r="B81">
+        <v>0.01</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0.5</v>
+      </c>
+      <c r="E81">
+        <v>0.01</v>
+      </c>
+      <c r="F81">
+        <v>0.49284015252336399</v>
+      </c>
+      <c r="G81">
+        <v>0.428327747479406</v>
+      </c>
+      <c r="H81">
+        <v>0.95030916422702705</v>
+      </c>
+      <c r="I81">
+        <v>0.64492816744908199</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="M81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A82" s="3">
+        <v>2079</v>
+      </c>
+      <c r="B82">
+        <v>0.01</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0.5</v>
+      </c>
+      <c r="E82">
+        <v>0.01</v>
+      </c>
+      <c r="F82">
+        <v>0.50819983401869095</v>
+      </c>
+      <c r="G82">
+        <v>0.44569685673805598</v>
+      </c>
+      <c r="H82">
+        <v>0.95437730841905799</v>
+      </c>
+      <c r="I82">
+        <v>0.65611250244430697</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+      <c r="M82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>2080</v>
+      </c>
+      <c r="B83">
+        <v>0.01</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0.5</v>
+      </c>
+      <c r="E83">
+        <v>0.01</v>
+      </c>
+      <c r="F83">
+        <v>0.52388443257676898</v>
+      </c>
+      <c r="G83">
+        <v>0.46351335373028901</v>
+      </c>
+      <c r="H83">
+        <v>0.95830455412291604</v>
+      </c>
+      <c r="I83">
+        <v>0.66733347954168998</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>1</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="M83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A84" s="3">
+        <v>2081</v>
+      </c>
+      <c r="B84">
+        <v>0.01</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0.5</v>
+      </c>
+      <c r="E84">
+        <v>0.01</v>
+      </c>
+      <c r="F84">
+        <v>0.53989017612817003</v>
+      </c>
+      <c r="G84">
+        <v>0.48176828084725798</v>
+      </c>
+      <c r="H84">
+        <v>0.96208618654270295</v>
+      </c>
+      <c r="I84">
+        <v>0.67859145727179004</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84">
+        <v>1</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+      <c r="M84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>2082</v>
+      </c>
+      <c r="B85">
+        <v>0.01</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0.5</v>
+      </c>
+      <c r="E85">
+        <v>0.01</v>
+      </c>
+      <c r="F85">
+        <v>0.55621329260347097</v>
+      </c>
+      <c r="G85">
+        <v>0.50045268048011204</v>
+      </c>
+      <c r="H85">
+        <v>0.96571749088252001</v>
+      </c>
+      <c r="I85">
+        <v>0.68988679416516296</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="L85">
+        <v>1</v>
+      </c>
+      <c r="M85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A86" s="3">
+        <v>2083</v>
+      </c>
+      <c r="B86">
+        <v>0.01</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0.5</v>
+      </c>
+      <c r="E86">
+        <v>0.01</v>
+      </c>
+      <c r="F86">
+        <v>0.57285000993324398</v>
+      </c>
+      <c r="G86">
+        <v>0.51955759502000398</v>
+      </c>
+      <c r="H86">
+        <v>0.96919375234646798</v>
+      </c>
+      <c r="I86">
+        <v>0.70121984875236598</v>
+      </c>
+      <c r="J86">
+        <v>1</v>
+      </c>
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+      <c r="M86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>2084</v>
+      </c>
+      <c r="B87">
+        <v>0.01</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0.5</v>
+      </c>
+      <c r="E87">
+        <v>0.01</v>
+      </c>
+      <c r="F87">
+        <v>0.58979655604806402</v>
+      </c>
+      <c r="G87">
+        <v>0.53907406685808401</v>
+      </c>
+      <c r="H87">
+        <v>0.97251025613864905</v>
+      </c>
+      <c r="I87">
+        <v>0.71259097956395401</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+      <c r="L87">
+        <v>1</v>
+      </c>
+      <c r="M87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A88" s="3">
+        <v>2085</v>
+      </c>
+      <c r="B88">
+        <v>0.01</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0.5</v>
+      </c>
+      <c r="E88">
+        <v>0.01</v>
+      </c>
+      <c r="F88">
+        <v>0.60704915887850397</v>
+      </c>
+      <c r="G88">
+        <v>0.55899313838550202</v>
+      </c>
+      <c r="H88">
+        <v>0.97566228746316397</v>
+      </c>
+      <c r="I88">
+        <v>0.72400054513048395</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88">
+        <v>1</v>
+      </c>
+      <c r="M88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>2086</v>
+      </c>
+      <c r="B89">
+        <v>0.01</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0.5</v>
+      </c>
+      <c r="E89">
+        <v>0.01</v>
+      </c>
+      <c r="F89">
+        <v>0.62460404635514</v>
+      </c>
+      <c r="G89">
+        <v>0.57930585199341</v>
+      </c>
+      <c r="H89">
+        <v>0.97864513152411503</v>
+      </c>
+      <c r="I89">
+        <v>0.73544890398251395</v>
+      </c>
+      <c r="J89">
+        <v>1</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89">
+        <v>1</v>
+      </c>
+      <c r="M89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A90" s="3">
+        <v>2087</v>
+      </c>
+      <c r="B90">
+        <v>0.01</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0.5</v>
+      </c>
+      <c r="E90">
+        <v>0.01</v>
+      </c>
+      <c r="F90">
+        <v>0.64245744640854396</v>
+      </c>
+      <c r="G90">
+        <v>0.60000325007295796</v>
+      </c>
+      <c r="H90">
+        <v>0.98145407352560299</v>
+      </c>
+      <c r="I90">
+        <v>0.74693641465059901</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="L90">
+        <v>1</v>
+      </c>
+      <c r="M90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>2088</v>
+      </c>
+      <c r="B91">
+        <v>0.01</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0.5</v>
+      </c>
+      <c r="E91">
+        <v>0.01</v>
+      </c>
+      <c r="F91">
+        <v>0.66060558696929195</v>
+      </c>
+      <c r="G91">
+        <v>0.621076375015297</v>
+      </c>
+      <c r="H91">
+        <v>0.98408439867173003</v>
+      </c>
+      <c r="I91">
+        <v>0.75846343566529695</v>
+      </c>
+      <c r="J91">
+        <v>1</v>
+      </c>
+      <c r="K91">
+        <v>1</v>
+      </c>
+      <c r="L91">
+        <v>1</v>
+      </c>
+      <c r="M91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A92" s="3">
+        <v>2089</v>
+      </c>
+      <c r="B92">
+        <v>0.01</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0.5</v>
+      </c>
+      <c r="E92">
+        <v>0.01</v>
+      </c>
+      <c r="F92">
+        <v>0.67904469596795702</v>
+      </c>
+      <c r="G92">
+        <v>0.64251626921157901</v>
+      </c>
+      <c r="H92">
+        <v>0.98653139216659702</v>
+      </c>
+      <c r="I92">
+        <v>0.770030325557162</v>
+      </c>
+      <c r="J92">
+        <v>1</v>
+      </c>
+      <c r="K92">
+        <v>1</v>
+      </c>
+      <c r="L92">
+        <v>1</v>
+      </c>
+      <c r="M92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>2090</v>
+      </c>
+      <c r="B93">
+        <v>0.01</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0.5</v>
+      </c>
+      <c r="E93">
+        <v>0.01</v>
+      </c>
+      <c r="F93">
+        <v>0.69777100133511305</v>
+      </c>
+      <c r="G93">
+        <v>0.66431397505295298</v>
+      </c>
+      <c r="H93">
+        <v>0.98879033921430504</v>
+      </c>
+      <c r="I93">
+        <v>0.78163744285675396</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="K93">
+        <v>1</v>
+      </c>
+      <c r="L93">
+        <v>1</v>
+      </c>
+      <c r="M93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A94" s="3">
+        <v>2091</v>
+      </c>
+      <c r="B94">
+        <v>0.01</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0.5</v>
+      </c>
+      <c r="E94">
+        <v>0.01</v>
+      </c>
+      <c r="F94">
+        <v>0.71678073100133499</v>
+      </c>
+      <c r="G94">
+        <v>0.68646053493057102</v>
+      </c>
+      <c r="H94">
+        <v>0.99085652501895705</v>
+      </c>
+      <c r="I94">
+        <v>0.79328514609462697</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+      <c r="K94">
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <v>1</v>
+      </c>
+      <c r="M94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>2092</v>
+      </c>
+      <c r="B95">
+        <v>0.01</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0.5</v>
+      </c>
+      <c r="E95">
+        <v>0.01</v>
+      </c>
+      <c r="F95">
+        <v>0.73607011289719604</v>
+      </c>
+      <c r="G95">
+        <v>0.70894699123558402</v>
+      </c>
+      <c r="H95">
+        <v>0.99272523478465302</v>
+      </c>
+      <c r="I95">
+        <v>0.80497379380133804</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+      <c r="K95">
+        <v>1</v>
+      </c>
+      <c r="L95">
+        <v>1</v>
+      </c>
+      <c r="M95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A96" s="3">
+        <v>2093</v>
+      </c>
+      <c r="B96">
+        <v>0.01</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0.5</v>
+      </c>
+      <c r="E96">
+        <v>0.01</v>
+      </c>
+      <c r="F96">
+        <v>0.75563537495327104</v>
+      </c>
+      <c r="G96">
+        <v>0.73176438635914298</v>
+      </c>
+      <c r="H96">
+        <v>0.99439175371549504</v>
+      </c>
+      <c r="I96">
+        <v>0.81670374450744498</v>
+      </c>
+      <c r="J96">
+        <v>1</v>
+      </c>
+      <c r="K96">
+        <v>1</v>
+      </c>
+      <c r="L96">
+        <v>1</v>
+      </c>
+      <c r="M96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>2094</v>
+      </c>
+      <c r="B97">
+        <v>0.01</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0.5</v>
+      </c>
+      <c r="E97">
+        <v>0.01</v>
+      </c>
+      <c r="F97">
+        <v>0.77547274510013298</v>
+      </c>
+      <c r="G97">
+        <v>0.75490376269239801</v>
+      </c>
+      <c r="H97">
+        <v>0.99585136701558497</v>
+      </c>
+      <c r="I97">
+        <v>0.82847535674350303</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+      <c r="L97">
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A98" s="3">
+        <v>2095</v>
+      </c>
+      <c r="B98">
+        <v>0.01</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0.5</v>
+      </c>
+      <c r="E98">
+        <v>0.01</v>
+      </c>
+      <c r="F98">
+        <v>0.79557845126835702</v>
+      </c>
+      <c r="G98">
+        <v>0.77835616262649998</v>
+      </c>
+      <c r="H98">
+        <v>0.99709935988902298</v>
+      </c>
+      <c r="I98">
+        <v>0.84028898904006899</v>
+      </c>
+      <c r="J98">
+        <v>1</v>
+      </c>
+      <c r="K98">
+        <v>1</v>
+      </c>
+      <c r="L98">
+        <v>1</v>
+      </c>
+      <c r="M98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>2096</v>
+      </c>
+      <c r="B99">
+        <v>0.01</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0.5</v>
+      </c>
+      <c r="E99">
+        <v>0.01</v>
+      </c>
+      <c r="F99">
+        <v>0.81594872138851804</v>
+      </c>
+      <c r="G99">
+        <v>0.80211262855260002</v>
+      </c>
+      <c r="H99">
+        <v>0.99813101753991196</v>
+      </c>
+      <c r="I99">
+        <v>0.85214499992769999</v>
+      </c>
+      <c r="J99">
+        <v>1</v>
+      </c>
+      <c r="K99">
+        <v>1</v>
+      </c>
+      <c r="L99">
+        <v>1</v>
+      </c>
+      <c r="M99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A100" s="3">
+        <v>2097</v>
+      </c>
+      <c r="B100">
+        <v>0.01</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0.5</v>
+      </c>
+      <c r="E100">
+        <v>0.01</v>
+      </c>
+      <c r="F100">
+        <v>0.83657978339118799</v>
+      </c>
+      <c r="G100">
+        <v>0.826164202861849</v>
+      </c>
+      <c r="H100">
+        <v>0.99894162517235296</v>
+      </c>
+      <c r="I100">
+        <v>0.86404374793695105</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="L100">
+        <v>1</v>
+      </c>
+      <c r="M100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>2098</v>
+      </c>
+      <c r="B101">
+        <v>0.01</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0.5</v>
+      </c>
+      <c r="E101">
+        <v>0.01</v>
+      </c>
+      <c r="F101">
+        <v>0.85746786520694196</v>
+      </c>
+      <c r="G101">
+        <v>0.85050192794539903</v>
+      </c>
+      <c r="H101">
+        <v>0.99952646799044598</v>
+      </c>
+      <c r="I101">
+        <v>0.87598559159838096</v>
+      </c>
+      <c r="J101">
+        <v>1</v>
+      </c>
+      <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="L101">
+        <v>1</v>
+      </c>
+      <c r="M101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A102" s="3">
+        <v>2099</v>
+      </c>
+      <c r="B102">
+        <v>0.01</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0.5</v>
+      </c>
+      <c r="E102">
+        <v>0.01</v>
+      </c>
+      <c r="F102">
+        <v>0.87860919476635502</v>
+      </c>
+      <c r="G102">
+        <v>0.875116846194398</v>
+      </c>
+      <c r="H102">
+        <v>0.99988083119829496</v>
+      </c>
+      <c r="I102">
+        <v>0.88797088944254499</v>
+      </c>
+      <c r="J102">
+        <v>1</v>
+      </c>
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102">
+        <v>1</v>
+      </c>
+      <c r="M102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>2100</v>
+      </c>
+      <c r="B103">
+        <v>0.01</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0.5</v>
+      </c>
+      <c r="E103">
+        <v>0.01</v>
+      </c>
+      <c r="F103">
+        <v>0.9</v>
+      </c>
+      <c r="G103">
+        <v>0.9</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <v>0.89999999999999902</v>
+      </c>
+      <c r="J103">
+        <v>1</v>
+      </c>
+      <c r="K103">
+        <v>1</v>
+      </c>
+      <c r="L103">
+        <v>1</v>
+      </c>
+      <c r="M103">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>